<commit_message>
JAVA DOC Remain entities VIews ghealth
</commit_message>
<xml_diff>
--- a/GHealthProject/Progress.xlsx
+++ b/GHealthProject/Progress.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aj_pa\Repositories\labratoryCode\GHealthProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abu Nawaf\labratoryCode\GHealthProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>Bolous</t>
   </si>
@@ -232,13 +232,67 @@
   </si>
   <si>
     <t>Test Jars on computers</t>
+  </si>
+  <si>
+    <t>ClientUI</t>
+  </si>
+  <si>
+    <t>RequestInformationUI</t>
+  </si>
+  <si>
+    <t>Userscontroller</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>UITest</t>
+  </si>
+  <si>
+    <t>Entities&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Referral</t>
+  </si>
+  <si>
+    <t>VIEW&lt;&lt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>doctor (1)</t>
+  </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Muhmad</t>
+  </si>
+  <si>
+    <t>ghealth.Utils</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>DoctorCOmprator</t>
+  </si>
+  <si>
+    <t>Request</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +319,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -300,6 +368,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -318,7 +389,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1002,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,9 +1084,13 @@
     <col min="3" max="3" width="26.5703125" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1025,15 +1100,17 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
@@ -1043,8 +1120,14 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>10</v>
@@ -1054,8 +1137,14 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
         <v>10</v>
@@ -1065,8 +1154,14 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1075,8 +1170,14 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1085,8 +1186,14 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>63</v>
       </c>
@@ -1096,22 +1203,44 @@
       <c r="E9" s="5"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>0</v>
       </c>
@@ -1119,8 +1248,14 @@
         <v>65</v>
       </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
@@ -1129,8 +1264,14 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1280,14 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>0</v>
       </c>
@@ -1149,14 +1296,20 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -1165,8 +1318,12 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>67</v>
       </c>
@@ -1175,26 +1332,64 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
+      <c r="G23" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed java doc for classes
</commit_message>
<xml_diff>
--- a/GHealthProject/Progress.xlsx
+++ b/GHealthProject/Progress.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="89">
   <si>
     <t>Bolous</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t xml:space="preserve">checks valid fields </t>
+  </si>
+  <si>
+    <t>LaboratoryUI</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -363,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -374,6 +383,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="F22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="G9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,8 +1138,8 @@
       <c r="G4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>10</v>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1140,10 +1152,10 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1173,10 +1185,10 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1205,6 +1217,12 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="1"/>
+      <c r="G9" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
@@ -1236,10 +1254,10 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1301,10 +1319,10 @@
         <v>87</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1337,10 +1355,10 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" t="s">
+      <c r="G20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1352,6 +1370,9 @@
       <c r="G21" t="s">
         <v>50</v>
       </c>
+      <c r="H21" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>

</xml_diff>